<commit_message>
Update report.html with new test results and statistics for addIncomeTest
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/AddIncome.xlsx
+++ b/ProjectTest65/Excel/AddIncome.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F722D8C-B6C3-4D82-9B5A-59AD9DDB3039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10EF341-2ECE-4E66-A124-077AB6CD5B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Execute</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>ระบบไม่ได้ดักalertในส่วนถ้าไม่ได้กรอกจำนวนเป็นตัวเลขเท่านั้น</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -248,6 +251,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
@@ -256,7 +268,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -312,6 +324,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -625,8 +640,8 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -638,6 +653,7 @@
     <col min="5" max="5" width="30.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="19.5" customHeight="1">
@@ -853,6 +869,9 @@
       <c r="H7" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="I7" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
@@ -882,6 +901,7 @@
       <c r="H8" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="I8" s="23"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -911,6 +931,7 @@
       <c r="H9" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="I9" s="23"/>
       <c r="K9" s="22" t="s">
         <v>7</v>
       </c>
@@ -942,6 +963,7 @@
       <c r="H10" s="12" t="s">
         <v>20</v>
       </c>
+      <c r="I10" s="23"/>
       <c r="K10" s="20" t="s">
         <v>16</v>
       </c>
@@ -999,11 +1021,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K9:M9"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="K3:M3"/>
+    <mergeCell ref="I7:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>